<commit_message>
add cleaned seasonal c budget dataset, for ms and to merge with rest of tt work
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_SampleList-Solid_PPMS_v2023.xlsx
+++ b/data_log_sheets/TT24_SampleList-Solid_PPMS_v2023.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700D3244-CD9F-C94D-A4FA-B7FD99BF4CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2478786A-474A-7044-814A-F176AF76F771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC3A" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="33240" windowHeight="26940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="760" windowWidth="29020" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample List" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="440">
   <si>
     <t>13C, 15N</t>
   </si>
@@ -1352,6 +1352,12 @@
   </si>
   <si>
     <t>TT24_c_budget</t>
+  </si>
+  <si>
+    <t>P239588</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -2273,7 +2279,7 @@
   <dimension ref="A1:V1082"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2358,7 +2364,9 @@
       <c r="F4" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="74"/>
+      <c r="G4" s="74" t="s">
+        <v>438</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>188</v>
       </c>
@@ -2397,7 +2405,9 @@
       <c r="F6" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="G6" s="74"/>
+      <c r="G6" s="82" t="s">
+        <v>439</v>
+      </c>
       <c r="H6" s="75"/>
       <c r="I6" s="75"/>
       <c r="J6" s="75"/>
@@ -21333,7 +21343,7 @@
   </hyperlinks>
   <printOptions gridLines="1" gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="65" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
@@ -21966,6 +21976,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4CA004E70677E4D99DC762DFA1525D5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d0c3d59bf049a935e5f23360284eb36">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1eca514-60b3-4f5f-bd08-312baea136dd" xmlns:ns4="7f030698-0bc5-4997-8228-9217a142d4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bf59c473c335b8c9872e114636300839" ns3:_="" ns4:_="">
     <xsd:import namespace="a1eca514-60b3-4f5f-bd08-312baea136dd"/>
@@ -22188,22 +22213,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B46AABD-5B26-4236-9388-95A0F076CA7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a1eca514-60b3-4f5f-bd08-312baea136dd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7f030698-0bc5-4997-8228-9217a142d4e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5E342A6-EA00-4982-8621-46062975783E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{691BC5C0-30F6-4FC6-9FEA-0E2216C26930}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22220,29 +22255,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5E342A6-EA00-4982-8621-46062975783E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B46AABD-5B26-4236-9388-95A0F076CA7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1eca514-60b3-4f5f-bd08-312baea136dd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7f030698-0bc5-4997-8228-9217a142d4e9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>